<commit_message>
created records (drink, accessory), attribut color to Drink added in table_model
</commit_message>
<xml_diff>
--- a/Database/table_model.xlsx
+++ b/Database/table_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WineProject\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C97D8B-F77C-4DBE-8F36-C189DFFBB7B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851044E3-AA97-4CBB-930B-9B7064520534}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9CF1DE83-ACB3-4D14-928D-F8B5574C6510}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9CF1DE83-ACB3-4D14-928D-F8B5574C6510}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="96">
   <si>
     <t>PK</t>
   </si>
@@ -304,6 +304,21 @@
   </si>
   <si>
     <t>4,2()</t>
+  </si>
+  <si>
+    <t>residualSugar('bone dry', 'dry', 'off-dry', 'medium-sweet', 'sweet')</t>
+  </si>
+  <si>
+    <t>in litre</t>
+  </si>
+  <si>
+    <t>in percent</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>color('white', 'red', 'rosé')</t>
   </si>
 </sst>
 </file>
@@ -691,24 +706,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAA5F66-C1C3-4459-98AD-A0EE38B9A547}">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.1796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" style="2"/>
-    <col min="5" max="5" width="13.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="43.54296875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="49.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="2"/>
+    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="79.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>73</v>
       </c>
@@ -731,7 +746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -740,7 +755,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -760,7 +775,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -774,7 +789,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -788,7 +803,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -802,7 +817,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -819,7 +834,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -828,7 +843,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -848,7 +863,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
@@ -862,7 +877,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
@@ -876,7 +891,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
@@ -887,7 +902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
@@ -901,7 +916,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -918,7 +933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
@@ -932,7 +947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -941,7 +956,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -961,7 +976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
@@ -978,7 +993,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
@@ -992,7 +1007,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1006,7 +1021,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1015,7 +1030,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1035,7 +1050,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>20</v>
@@ -1052,7 +1067,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
@@ -1071,7 +1086,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>12</v>
@@ -1088,7 +1103,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>13</v>
@@ -1107,7 +1122,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>7</v>
@@ -1124,7 +1139,7 @@
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1133,7 +1148,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>19</v>
       </c>
@@ -1154,7 +1169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>20</v>
       </c>
@@ -1168,7 +1183,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
@@ -1182,7 +1197,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>22</v>
       </c>
@@ -1196,7 +1211,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>23</v>
       </c>
@@ -1210,7 +1225,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>30</v>
       </c>
@@ -1224,7 +1239,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1233,7 +1248,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
@@ -1253,7 +1268,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>34</v>
       </c>
@@ -1270,7 +1285,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>35</v>
       </c>
@@ -1284,7 +1299,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1293,7 +1308,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -1313,7 +1328,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>48</v>
       </c>
@@ -1327,18 +1342,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>71</v>
       </c>
@@ -1351,22 +1366,25 @@
       <c r="E43" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G43" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G44" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>51</v>
       </c>
@@ -1379,316 +1397,322 @@
       <c r="E45" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G45" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" s="2" t="s">
+      <c r="C47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="C49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B49" s="2" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="2">
+      <c r="C50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="2">
         <v>100</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B50" s="2" t="s">
+      <c r="E50" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B51" s="2" t="s">
+      <c r="E51" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F51" s="2" t="s">
+      <c r="C52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F53" s="2" t="s">
+      <c r="C54" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B54" s="2" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G54" s="2" t="s">
+      <c r="E55" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B55" s="2" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D55" s="2">
+      <c r="C56" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" s="2">
         <v>100</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B56" s="2" t="s">
+      <c r="E56" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F56" s="2" t="s">
+      <c r="C57" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F58" s="2" t="s">
+      <c r="C59" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B59" s="2" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B60" s="2" t="s">
+      <c r="E60" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="2">
+      <c r="C61" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="2">
         <v>5</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B61" s="2" t="s">
+      <c r="E61" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F61" s="2" t="s">
+      <c r="C62" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B62" s="2" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F62" s="2" t="s">
+      <c r="C63" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F64" s="2" t="s">
+      <c r="C65" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B65" s="2" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B66" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E66" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B67" s="2" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B68" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>81</v>
@@ -1697,45 +1721,59 @@
         <v>41</v>
       </c>
       <c r="G68" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B69" s="2" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B70" s="2" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F70" s="2" t="s">
+      <c r="C71" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B71" s="2" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F71" s="2" t="s">
+      <c r="C72" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>